<commit_message>
- added function to compute mean and cov from trajectories - added toggle switch to standard models
</commit_message>
<xml_diff>
--- a/pyssa/models/collection/stochastic_repressilator.xlsx
+++ b/pyssa/models/collection/stochastic_repressilator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christian/Documents/Code/pyssa/pyssa/models/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C5618D-41B2-EA42-AA05-5F70354CF85C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF9F2BF-891A-3C43-B663-77725A3B4118}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-42880" yWindow="4360" windowWidth="31240" windowHeight="20060" xr2:uid="{EC645E34-98D1-AB4F-B87A-DEAC07020CA2}"/>
   </bookViews>
@@ -514,8 +514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EFA4861-CF3A-494C-89B9-FB1324E56C6E}">
   <dimension ref="A3:P90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="G76" sqref="G76"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="G75" sqref="G75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1090,7 +1090,7 @@
         <v>18</v>
       </c>
       <c r="B66" s="1">
-        <v>2.5000000000000001E-2</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1163,7 +1163,7 @@
         <v>27</v>
       </c>
       <c r="B75" s="1">
-        <v>2.5000000000000001E-2</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1236,7 +1236,7 @@
         <v>36</v>
       </c>
       <c r="B84" s="1">
-        <v>2.5000000000000001E-2</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="85" spans="1:2">

</xml_diff>